<commit_message>
added more data and report.txt to compose on
</commit_message>
<xml_diff>
--- a/Project2/report.xlsx
+++ b/Project2/report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanjay\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanjay\Documents\GitHub\COP5615-Projects\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3300,11 +3300,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="398061976"/>
-        <c:axId val="398059624"/>
+        <c:axId val="351923912"/>
+        <c:axId val="353585752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="398061976"/>
+        <c:axId val="351923912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3403,7 +3403,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="398059624"/>
+        <c:crossAx val="353585752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3411,7 +3411,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="398059624"/>
+        <c:axId val="353585752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3518,7 +3518,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="398061976"/>
+        <c:crossAx val="351923912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6012,9 +6012,6 @@
                 <c:pt idx="46">
                   <c:v>0.36326120658093475</c:v>
                 </c:pt>
-                <c:pt idx="49">
-                  <c:v>1.5</c:v>
-                </c:pt>
                 <c:pt idx="55">
                   <c:v>0.3698328965297053</c:v>
                 </c:pt>
@@ -6518,12 +6515,12 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="398053744"/>
-        <c:axId val="398054136"/>
+        <c:axId val="353580656"/>
+        <c:axId val="353581048"/>
         <c:extLst/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="398053744"/>
+        <c:axId val="353580656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6622,7 +6619,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="398054136"/>
+        <c:crossAx val="353581048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6630,7 +6627,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="398054136"/>
+        <c:axId val="353581048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6737,7 +6734,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="398053744"/>
+        <c:crossAx val="353580656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8234,9 +8231,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K94" sqref="K94"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9204,9 +9201,6 @@
         <f>LOG10(2.63598)</f>
         <v>0.42094211080718119</v>
       </c>
-      <c r="N52">
-        <v>1.5</v>
-      </c>
       <c r="O52" s="10"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added more data for gossip imp2D
</commit_message>
<xml_diff>
--- a/Project2/report.xlsx
+++ b/Project2/report.xlsx
@@ -304,10 +304,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$125</c:f>
+              <c:f>Sheet1!$B$3:$B$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -651,30 +651,54 @@
                   <c:v>42875</c:v>
                 </c:pt>
                 <c:pt idx="114">
+                  <c:v>45369</c:v>
+                </c:pt>
+                <c:pt idx="115">
                   <c:v>50653</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="116">
+                  <c:v>55225</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>64000</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="118">
+                  <c:v>65025</c:v>
+                </c:pt>
+                <c:pt idx="119">
                   <c:v>74088</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="120">
+                  <c:v>75076</c:v>
+                </c:pt>
+                <c:pt idx="121">
                   <c:v>85184</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="122">
+                  <c:v>85264</c:v>
+                </c:pt>
+                <c:pt idx="123">
                   <c:v>91125</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="124">
+                  <c:v>95481</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>100489</c:v>
+                </c:pt>
+                <c:pt idx="126">
                   <c:v>103823</c:v>
                 </c:pt>
-                <c:pt idx="120">
-                  <c:v>100489</c:v>
-                </c:pt>
-                <c:pt idx="121">
+                <c:pt idx="127">
+                  <c:v>105625</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>205209</c:v>
+                </c:pt>
+                <c:pt idx="129">
                   <c:v>205379</c:v>
                 </c:pt>
-                <c:pt idx="122">
+                <c:pt idx="130">
                   <c:v>300763</c:v>
                 </c:pt>
               </c:numCache>
@@ -682,10 +706,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$125</c:f>
+              <c:f>Sheet1!$C$3:$C$133</c:f>
               <c:numCache>
                 <c:formatCode>@</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="5" formatCode="General">
                   <c:v>0.52922599999999997</c:v>
                 </c:pt>
@@ -825,10 +849,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$125</c:f>
+              <c:f>Sheet1!$B$3:$B$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1172,30 +1196,54 @@
                   <c:v>42875</c:v>
                 </c:pt>
                 <c:pt idx="114">
+                  <c:v>45369</c:v>
+                </c:pt>
+                <c:pt idx="115">
                   <c:v>50653</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="116">
+                  <c:v>55225</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>64000</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="118">
+                  <c:v>65025</c:v>
+                </c:pt>
+                <c:pt idx="119">
                   <c:v>74088</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="120">
+                  <c:v>75076</c:v>
+                </c:pt>
+                <c:pt idx="121">
                   <c:v>85184</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="122">
+                  <c:v>85264</c:v>
+                </c:pt>
+                <c:pt idx="123">
                   <c:v>91125</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="124">
+                  <c:v>95481</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>100489</c:v>
+                </c:pt>
+                <c:pt idx="126">
                   <c:v>103823</c:v>
                 </c:pt>
-                <c:pt idx="120">
-                  <c:v>100489</c:v>
-                </c:pt>
-                <c:pt idx="121">
+                <c:pt idx="127">
+                  <c:v>105625</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>205209</c:v>
+                </c:pt>
+                <c:pt idx="129">
                   <c:v>205379</c:v>
                 </c:pt>
-                <c:pt idx="122">
+                <c:pt idx="130">
                   <c:v>300763</c:v>
                 </c:pt>
               </c:numCache>
@@ -1203,10 +1251,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$125</c:f>
+              <c:f>Sheet1!$D$3:$D$133</c:f>
               <c:numCache>
                 <c:formatCode>@</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="5" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1334,10 +1382,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$125</c:f>
+              <c:f>Sheet1!$B$3:$B$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1681,30 +1729,54 @@
                   <c:v>42875</c:v>
                 </c:pt>
                 <c:pt idx="114">
+                  <c:v>45369</c:v>
+                </c:pt>
+                <c:pt idx="115">
                   <c:v>50653</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="116">
+                  <c:v>55225</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>64000</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="118">
+                  <c:v>65025</c:v>
+                </c:pt>
+                <c:pt idx="119">
                   <c:v>74088</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="120">
+                  <c:v>75076</c:v>
+                </c:pt>
+                <c:pt idx="121">
                   <c:v>85184</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="122">
+                  <c:v>85264</c:v>
+                </c:pt>
+                <c:pt idx="123">
                   <c:v>91125</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="124">
+                  <c:v>95481</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>100489</c:v>
+                </c:pt>
+                <c:pt idx="126">
                   <c:v>103823</c:v>
                 </c:pt>
-                <c:pt idx="120">
-                  <c:v>100489</c:v>
-                </c:pt>
-                <c:pt idx="121">
+                <c:pt idx="127">
+                  <c:v>105625</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>205209</c:v>
+                </c:pt>
+                <c:pt idx="129">
                   <c:v>205379</c:v>
                 </c:pt>
-                <c:pt idx="122">
+                <c:pt idx="130">
                   <c:v>300763</c:v>
                 </c:pt>
               </c:numCache>
@@ -1712,10 +1784,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$125</c:f>
+              <c:f>Sheet1!$E$3:$E$133</c:f>
               <c:numCache>
                 <c:formatCode>@</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="5" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1888,10 +1960,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$125</c:f>
+              <c:f>Sheet1!$B$3:$B$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2235,30 +2307,54 @@
                   <c:v>42875</c:v>
                 </c:pt>
                 <c:pt idx="114">
+                  <c:v>45369</c:v>
+                </c:pt>
+                <c:pt idx="115">
                   <c:v>50653</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="116">
+                  <c:v>55225</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>64000</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="118">
+                  <c:v>65025</c:v>
+                </c:pt>
+                <c:pt idx="119">
                   <c:v>74088</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="120">
+                  <c:v>75076</c:v>
+                </c:pt>
+                <c:pt idx="121">
                   <c:v>85184</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="122">
+                  <c:v>85264</c:v>
+                </c:pt>
+                <c:pt idx="123">
                   <c:v>91125</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="124">
+                  <c:v>95481</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>100489</c:v>
+                </c:pt>
+                <c:pt idx="126">
                   <c:v>103823</c:v>
                 </c:pt>
-                <c:pt idx="120">
-                  <c:v>100489</c:v>
-                </c:pt>
-                <c:pt idx="121">
+                <c:pt idx="127">
+                  <c:v>105625</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>205209</c:v>
+                </c:pt>
+                <c:pt idx="129">
                   <c:v>205379</c:v>
                 </c:pt>
-                <c:pt idx="122">
+                <c:pt idx="130">
                   <c:v>300763</c:v>
                 </c:pt>
               </c:numCache>
@@ -2266,10 +2362,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$125</c:f>
+              <c:f>Sheet1!$G$3:$G$133</c:f>
               <c:numCache>
                 <c:formatCode>@</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="5" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2397,10 +2493,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$125</c:f>
+              <c:f>Sheet1!$B$3:$B$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2744,30 +2840,54 @@
                   <c:v>42875</c:v>
                 </c:pt>
                 <c:pt idx="114">
+                  <c:v>45369</c:v>
+                </c:pt>
+                <c:pt idx="115">
                   <c:v>50653</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="116">
+                  <c:v>55225</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>64000</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="118">
+                  <c:v>65025</c:v>
+                </c:pt>
+                <c:pt idx="119">
                   <c:v>74088</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="120">
+                  <c:v>75076</c:v>
+                </c:pt>
+                <c:pt idx="121">
                   <c:v>85184</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="122">
+                  <c:v>85264</c:v>
+                </c:pt>
+                <c:pt idx="123">
                   <c:v>91125</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="124">
+                  <c:v>95481</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>100489</c:v>
+                </c:pt>
+                <c:pt idx="126">
                   <c:v>103823</c:v>
                 </c:pt>
-                <c:pt idx="120">
-                  <c:v>100489</c:v>
-                </c:pt>
-                <c:pt idx="121">
+                <c:pt idx="127">
+                  <c:v>105625</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>205209</c:v>
+                </c:pt>
+                <c:pt idx="129">
                   <c:v>205379</c:v>
                 </c:pt>
-                <c:pt idx="122">
+                <c:pt idx="130">
                   <c:v>300763</c:v>
                 </c:pt>
               </c:numCache>
@@ -2775,10 +2895,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$125</c:f>
+              <c:f>Sheet1!$H$3:$H$133</c:f>
               <c:numCache>
                 <c:formatCode>@</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="6" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2818,28 +2938,28 @@
                 <c:pt idx="113" formatCode="General">
                   <c:v>3.8520599999999998</c:v>
                 </c:pt>
-                <c:pt idx="114" formatCode="General">
+                <c:pt idx="115" formatCode="General">
                   <c:v>3.97126</c:v>
                 </c:pt>
-                <c:pt idx="115" formatCode="General">
+                <c:pt idx="117" formatCode="General">
                   <c:v>4.2911099999999998</c:v>
                 </c:pt>
-                <c:pt idx="116" formatCode="General">
+                <c:pt idx="119" formatCode="General">
                   <c:v>4.4571699999999996</c:v>
                 </c:pt>
-                <c:pt idx="117" formatCode="General">
+                <c:pt idx="121" formatCode="General">
                   <c:v>4.5895700000000001</c:v>
                 </c:pt>
-                <c:pt idx="118" formatCode="General">
+                <c:pt idx="123" formatCode="General">
                   <c:v>4.6817700000000002</c:v>
                 </c:pt>
-                <c:pt idx="119" formatCode="General">
+                <c:pt idx="126" formatCode="General">
                   <c:v>4.7963300000000002</c:v>
                 </c:pt>
-                <c:pt idx="121" formatCode="General">
+                <c:pt idx="129" formatCode="General">
                   <c:v>5.67401</c:v>
                 </c:pt>
-                <c:pt idx="122" formatCode="General">
+                <c:pt idx="130" formatCode="General">
                   <c:v>6.59</c:v>
                 </c:pt>
               </c:numCache>
@@ -2879,10 +2999,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$125</c:f>
+              <c:f>Sheet1!$B$3:$B$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -3226,30 +3346,54 @@
                   <c:v>42875</c:v>
                 </c:pt>
                 <c:pt idx="114">
+                  <c:v>45369</c:v>
+                </c:pt>
+                <c:pt idx="115">
                   <c:v>50653</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="116">
+                  <c:v>55225</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>64000</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="118">
+                  <c:v>65025</c:v>
+                </c:pt>
+                <c:pt idx="119">
                   <c:v>74088</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="120">
+                  <c:v>75076</c:v>
+                </c:pt>
+                <c:pt idx="121">
                   <c:v>85184</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="122">
+                  <c:v>85264</c:v>
+                </c:pt>
+                <c:pt idx="123">
                   <c:v>91125</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="124">
+                  <c:v>95481</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>100489</c:v>
+                </c:pt>
+                <c:pt idx="126">
                   <c:v>103823</c:v>
                 </c:pt>
-                <c:pt idx="120">
-                  <c:v>100489</c:v>
-                </c:pt>
-                <c:pt idx="121">
+                <c:pt idx="127">
+                  <c:v>105625</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>205209</c:v>
+                </c:pt>
+                <c:pt idx="129">
                   <c:v>205379</c:v>
                 </c:pt>
-                <c:pt idx="122">
+                <c:pt idx="130">
                   <c:v>300763</c:v>
                 </c:pt>
               </c:numCache>
@@ -3257,10 +3401,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$125</c:f>
+              <c:f>Sheet1!$F$3:$F$133</c:f>
               <c:numCache>
                 <c:formatCode>@</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="5" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3300,11 +3444,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="351923912"/>
-        <c:axId val="353585752"/>
+        <c:axId val="355682448"/>
+        <c:axId val="355684016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="351923912"/>
+        <c:axId val="355682448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3403,7 +3547,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353585752"/>
+        <c:crossAx val="355684016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3411,7 +3555,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="353585752"/>
+        <c:axId val="355684016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3518,7 +3662,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351923912"/>
+        <c:crossAx val="355682448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3707,10 +3851,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$125</c:f>
+              <c:f>Sheet1!$B$3:$B$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -4054,30 +4198,54 @@
                   <c:v>42875</c:v>
                 </c:pt>
                 <c:pt idx="114">
+                  <c:v>45369</c:v>
+                </c:pt>
+                <c:pt idx="115">
                   <c:v>50653</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="116">
+                  <c:v>55225</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>64000</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="118">
+                  <c:v>65025</c:v>
+                </c:pt>
+                <c:pt idx="119">
                   <c:v>74088</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="120">
+                  <c:v>75076</c:v>
+                </c:pt>
+                <c:pt idx="121">
                   <c:v>85184</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="122">
+                  <c:v>85264</c:v>
+                </c:pt>
+                <c:pt idx="123">
                   <c:v>91125</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="124">
+                  <c:v>95481</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>100489</c:v>
+                </c:pt>
+                <c:pt idx="126">
                   <c:v>103823</c:v>
                 </c:pt>
-                <c:pt idx="120">
-                  <c:v>100489</c:v>
-                </c:pt>
-                <c:pt idx="121">
+                <c:pt idx="127">
+                  <c:v>105625</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>205209</c:v>
+                </c:pt>
+                <c:pt idx="129">
                   <c:v>205379</c:v>
                 </c:pt>
-                <c:pt idx="122">
+                <c:pt idx="130">
                   <c:v>300763</c:v>
                 </c:pt>
               </c:numCache>
@@ -4085,10 +4253,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$125</c:f>
+              <c:f>Sheet1!$J$3:$J$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4198,10 +4366,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$125</c:f>
+              <c:f>Sheet1!$B$3:$B$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -4545,30 +4713,54 @@
                   <c:v>42875</c:v>
                 </c:pt>
                 <c:pt idx="114">
+                  <c:v>45369</c:v>
+                </c:pt>
+                <c:pt idx="115">
                   <c:v>50653</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="116">
+                  <c:v>55225</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>64000</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="118">
+                  <c:v>65025</c:v>
+                </c:pt>
+                <c:pt idx="119">
                   <c:v>74088</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="120">
+                  <c:v>75076</c:v>
+                </c:pt>
+                <c:pt idx="121">
                   <c:v>85184</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="122">
+                  <c:v>85264</c:v>
+                </c:pt>
+                <c:pt idx="123">
                   <c:v>91125</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="124">
+                  <c:v>95481</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>100489</c:v>
+                </c:pt>
+                <c:pt idx="126">
                   <c:v>103823</c:v>
                 </c:pt>
-                <c:pt idx="120">
-                  <c:v>100489</c:v>
-                </c:pt>
-                <c:pt idx="121">
+                <c:pt idx="127">
+                  <c:v>105625</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>205209</c:v>
+                </c:pt>
+                <c:pt idx="129">
                   <c:v>205379</c:v>
                 </c:pt>
-                <c:pt idx="122">
+                <c:pt idx="130">
                   <c:v>300763</c:v>
                 </c:pt>
               </c:numCache>
@@ -4577,10 +4769,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$3:$K$125</c:f>
+              <c:f>Sheet1!$K$3:$K$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4644,7 +4836,7 @@
                 <c:pt idx="78">
                   <c:v>0.68652899999999994</c:v>
                 </c:pt>
-                <c:pt idx="120">
+                <c:pt idx="125">
                   <c:v>1.7864169999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -4685,10 +4877,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$125</c:f>
+              <c:f>Sheet1!$B$3:$B$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -5032,30 +5224,54 @@
                   <c:v>42875</c:v>
                 </c:pt>
                 <c:pt idx="114">
+                  <c:v>45369</c:v>
+                </c:pt>
+                <c:pt idx="115">
                   <c:v>50653</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="116">
+                  <c:v>55225</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>64000</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="118">
+                  <c:v>65025</c:v>
+                </c:pt>
+                <c:pt idx="119">
                   <c:v>74088</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="120">
+                  <c:v>75076</c:v>
+                </c:pt>
+                <c:pt idx="121">
                   <c:v>85184</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="122">
+                  <c:v>85264</c:v>
+                </c:pt>
+                <c:pt idx="123">
                   <c:v>91125</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="124">
+                  <c:v>95481</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>100489</c:v>
+                </c:pt>
+                <c:pt idx="126">
                   <c:v>103823</c:v>
                 </c:pt>
-                <c:pt idx="120">
-                  <c:v>100489</c:v>
-                </c:pt>
-                <c:pt idx="121">
+                <c:pt idx="127">
+                  <c:v>105625</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>205209</c:v>
+                </c:pt>
+                <c:pt idx="129">
                   <c:v>205379</c:v>
                 </c:pt>
-                <c:pt idx="122">
+                <c:pt idx="130">
                   <c:v>300763</c:v>
                 </c:pt>
               </c:numCache>
@@ -5063,10 +5279,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$125</c:f>
+              <c:f>Sheet1!$L$3:$L$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5118,22 +5334,22 @@
                 <c:pt idx="113">
                   <c:v>1.2287454240932043</c:v>
                 </c:pt>
-                <c:pt idx="114">
+                <c:pt idx="115">
                   <c:v>1.2884979902903051</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="117">
                   <c:v>1.4253534713915326</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="119">
                   <c:v>1.5133950383885446</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="121">
                   <c:v>1.5381709953493281</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="123">
                   <c:v>1.5331952633226487</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="126">
                   <c:v>2.1273930000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -5173,10 +5389,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$125</c:f>
+              <c:f>Sheet1!$B$3:$B$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -5520,30 +5736,54 @@
                   <c:v>42875</c:v>
                 </c:pt>
                 <c:pt idx="114">
+                  <c:v>45369</c:v>
+                </c:pt>
+                <c:pt idx="115">
                   <c:v>50653</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="116">
+                  <c:v>55225</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>64000</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="118">
+                  <c:v>65025</c:v>
+                </c:pt>
+                <c:pt idx="119">
                   <c:v>74088</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="120">
+                  <c:v>75076</c:v>
+                </c:pt>
+                <c:pt idx="121">
                   <c:v>85184</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="122">
+                  <c:v>85264</c:v>
+                </c:pt>
+                <c:pt idx="123">
                   <c:v>91125</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="124">
+                  <c:v>95481</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>100489</c:v>
+                </c:pt>
+                <c:pt idx="126">
                   <c:v>103823</c:v>
                 </c:pt>
-                <c:pt idx="120">
-                  <c:v>100489</c:v>
-                </c:pt>
-                <c:pt idx="121">
+                <c:pt idx="127">
+                  <c:v>105625</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>205209</c:v>
+                </c:pt>
+                <c:pt idx="129">
                   <c:v>205379</c:v>
                 </c:pt>
-                <c:pt idx="122">
+                <c:pt idx="130">
                   <c:v>300763</c:v>
                 </c:pt>
               </c:numCache>
@@ -5552,24 +5792,126 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$3:$M$125</c:f>
+              <c:f>Sheet1!$M$3:$M$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="24">
+                  <c:v>5.1077624318655465E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.27429547085506945</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.31112814891898549</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.24001602826950505</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.59047310143304821</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.47322371630407112</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.4905547082226831</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.51092040728651489</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.71568310922401601</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.60144380006461717</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.60131958343156777</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.92657495725097339</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.68199826607705716</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.98838304237963814</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.79032398723916319</c:v>
                 </c:pt>
                 <c:pt idx="78">
                   <c:v>0.73226599999999997</c:v>
                 </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.96013881417720048</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1.1614059479111796</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1.3908740176992924</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1.5451400690754507</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1.6739734897954159</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1.6956908927319843</c:v>
+                </c:pt>
                 <c:pt idx="120">
+                  <c:v>1.7020188598790844</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1.7417877636779429</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1.8891523319326773</c:v>
+                </c:pt>
+                <c:pt idx="125">
                   <c:v>1.875286</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1.8997290993698215</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>2.1757031874447921</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
@@ -5609,10 +5951,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$125</c:f>
+              <c:f>Sheet1!$B$3:$B$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -5956,30 +6298,54 @@
                   <c:v>42875</c:v>
                 </c:pt>
                 <c:pt idx="114">
+                  <c:v>45369</c:v>
+                </c:pt>
+                <c:pt idx="115">
                   <c:v>50653</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="116">
+                  <c:v>55225</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>64000</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="118">
+                  <c:v>65025</c:v>
+                </c:pt>
+                <c:pt idx="119">
                   <c:v>74088</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="120">
+                  <c:v>75076</c:v>
+                </c:pt>
+                <c:pt idx="121">
                   <c:v>85184</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="122">
+                  <c:v>85264</c:v>
+                </c:pt>
+                <c:pt idx="123">
                   <c:v>91125</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="124">
+                  <c:v>95481</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>100489</c:v>
+                </c:pt>
+                <c:pt idx="126">
                   <c:v>103823</c:v>
                 </c:pt>
-                <c:pt idx="120">
-                  <c:v>100489</c:v>
-                </c:pt>
-                <c:pt idx="121">
+                <c:pt idx="127">
+                  <c:v>105625</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>205209</c:v>
+                </c:pt>
+                <c:pt idx="129">
                   <c:v>205379</c:v>
                 </c:pt>
-                <c:pt idx="122">
+                <c:pt idx="130">
                   <c:v>300763</c:v>
                 </c:pt>
               </c:numCache>
@@ -5987,10 +6353,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$3:$N$125</c:f>
+              <c:f>Sheet1!$N$3:$N$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
@@ -6039,22 +6405,22 @@
                 <c:pt idx="113">
                   <c:v>1.2197187229049096</c:v>
                 </c:pt>
-                <c:pt idx="114">
+                <c:pt idx="115">
                   <c:v>1.3398066025952082</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="117">
                   <c:v>1.4710526659412606</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="119">
                   <c:v>1.5529771365445766</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="121">
                   <c:v>1.960211617165541</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="123">
                   <c:v>2.1669524184314453</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="126">
                   <c:v>2.499571</c:v>
                 </c:pt>
               </c:numCache>
@@ -6094,10 +6460,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$125</c:f>
+              <c:f>Sheet1!$B$3:$B$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -6441,30 +6807,54 @@
                   <c:v>42875</c:v>
                 </c:pt>
                 <c:pt idx="114">
+                  <c:v>45369</c:v>
+                </c:pt>
+                <c:pt idx="115">
                   <c:v>50653</c:v>
                 </c:pt>
-                <c:pt idx="115">
+                <c:pt idx="116">
+                  <c:v>55225</c:v>
+                </c:pt>
+                <c:pt idx="117">
                   <c:v>64000</c:v>
                 </c:pt>
-                <c:pt idx="116">
+                <c:pt idx="118">
+                  <c:v>65025</c:v>
+                </c:pt>
+                <c:pt idx="119">
                   <c:v>74088</c:v>
                 </c:pt>
-                <c:pt idx="117">
+                <c:pt idx="120">
+                  <c:v>75076</c:v>
+                </c:pt>
+                <c:pt idx="121">
                   <c:v>85184</c:v>
                 </c:pt>
-                <c:pt idx="118">
+                <c:pt idx="122">
+                  <c:v>85264</c:v>
+                </c:pt>
+                <c:pt idx="123">
                   <c:v>91125</c:v>
                 </c:pt>
-                <c:pt idx="119">
+                <c:pt idx="124">
+                  <c:v>95481</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>100489</c:v>
+                </c:pt>
+                <c:pt idx="126">
                   <c:v>103823</c:v>
                 </c:pt>
-                <c:pt idx="120">
-                  <c:v>100489</c:v>
-                </c:pt>
-                <c:pt idx="121">
+                <c:pt idx="127">
+                  <c:v>105625</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>205209</c:v>
+                </c:pt>
+                <c:pt idx="129">
                   <c:v>205379</c:v>
                 </c:pt>
-                <c:pt idx="122">
+                <c:pt idx="130">
                   <c:v>300763</c:v>
                 </c:pt>
               </c:numCache>
@@ -6472,10 +6862,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$3:$O$125</c:f>
+              <c:f>Sheet1!$O$3:$O$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="123"/>
+                <c:ptCount val="131"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -6515,12 +6905,12 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="353580656"/>
-        <c:axId val="353581048"/>
+        <c:axId val="355683232"/>
+        <c:axId val="357348168"/>
         <c:extLst/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="353580656"/>
+        <c:axId val="355683232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6619,7 +7009,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353581048"/>
+        <c:crossAx val="357348168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6627,7 +7017,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="353581048"/>
+        <c:axId val="357348168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6734,7 +7124,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353580656"/>
+        <c:crossAx val="355683232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8229,11 +8619,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O140"/>
+  <dimension ref="A1:O148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N54" sqref="N54"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L129" sqref="L129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8378,7 +8768,7 @@
       <c r="K8" s="8">
         <v>0</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8">
         <v>0</v>
       </c>
       <c r="O8" s="8"/>
@@ -8436,6 +8826,9 @@
         <v>0</v>
       </c>
       <c r="H11"/>
+      <c r="M11">
+        <v>0</v>
+      </c>
       <c r="O11" s="8"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -8470,6 +8863,9 @@
         <v>0</v>
       </c>
       <c r="H13"/>
+      <c r="M13">
+        <v>0</v>
+      </c>
       <c r="O13" s="8"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -8507,6 +8903,9 @@
       <c r="J15">
         <f>LOG10(3.787487)</f>
         <v>0.5783511508600766</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -8540,6 +8939,9 @@
         <v>0</v>
       </c>
       <c r="H17"/>
+      <c r="M17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18">
@@ -8582,6 +8984,9 @@
         <v>0</v>
       </c>
       <c r="H19"/>
+      <c r="M19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20">
@@ -8614,6 +9019,9 @@
         <v>0</v>
       </c>
       <c r="H21"/>
+      <c r="M21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22">
@@ -8646,6 +9054,9 @@
         <v>0</v>
       </c>
       <c r="H23"/>
+      <c r="M23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24">
@@ -8682,6 +9093,9 @@
       <c r="J25">
         <f>LOG10(14.44571)</f>
         <v>1.1597388920787564</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
@@ -8726,8 +9140,9 @@
       <c r="K27" s="8">
         <v>0</v>
       </c>
-      <c r="M27" s="8">
-        <v>0</v>
+      <c r="M27">
+        <f>LOG10(1.124806)</f>
+        <v>5.1077624318655465E-2</v>
       </c>
       <c r="O27">
         <f>LOG10(1.752106)</f>
@@ -8807,6 +9222,10 @@
       <c r="J31">
         <f>LOG10(13.909605)</f>
         <v>1.1433147972274107</v>
+      </c>
+      <c r="M31">
+        <f>LOG10(1.880595839)</f>
+        <v>0.27429547085506945</v>
       </c>
       <c r="O31" s="10"/>
     </row>
@@ -8856,6 +9275,9 @@
         <v>0.98421700000000001</v>
       </c>
       <c r="H34"/>
+      <c r="M34">
+        <v>0</v>
+      </c>
       <c r="O34" s="10"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
@@ -8913,6 +9335,10 @@
         <v>0.94357800000000003</v>
       </c>
       <c r="H37"/>
+      <c r="M37">
+        <f>LOG10(2.047048578)</f>
+        <v>0.31112814891898549</v>
+      </c>
       <c r="O37" s="10"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
@@ -8949,6 +9375,10 @@
         <v>1.2785599999999999</v>
       </c>
       <c r="H39"/>
+      <c r="M39">
+        <f>LOG10(1.737864966)</f>
+        <v>0.24001602826950505</v>
+      </c>
       <c r="O39" s="10"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
@@ -8998,6 +9428,10 @@
       <c r="K41">
         <f>LOG10(1.680372)</f>
         <v>0.22540543628727924</v>
+      </c>
+      <c r="M41">
+        <f>LOG10(3.894691847)</f>
+        <v>0.59047310143304821</v>
       </c>
       <c r="O41" s="10"/>
     </row>
@@ -9059,6 +9493,10 @@
         <v>1.722</v>
       </c>
       <c r="H44"/>
+      <c r="M44">
+        <f>LOG10(2.973197208)</f>
+        <v>0.47322371630407112</v>
+      </c>
       <c r="O44" s="10"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
@@ -9094,6 +9532,10 @@
       <c r="K46">
         <f>LOG10(3.56983)</f>
         <v>0.55264753493016572</v>
+      </c>
+      <c r="M46">
+        <f>LOG10(3.094245074)</f>
+        <v>0.4905547082226831</v>
       </c>
       <c r="O46" s="10"/>
     </row>
@@ -9269,6 +9711,10 @@
         <f>LOG10(2.79907)</f>
         <v>0.44701375957141287</v>
       </c>
+      <c r="M56">
+        <f>LOG10(3.242801814)</f>
+        <v>0.51092040728651489</v>
+      </c>
       <c r="O56" s="10"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
@@ -9375,6 +9821,10 @@
         <f>LOG10(6.125194)</f>
         <v>0.78711984843170846</v>
       </c>
+      <c r="M62">
+        <f>LOG10(5.196167105)</f>
+        <v>0.71568310922401601</v>
+      </c>
       <c r="O62" s="10"/>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
@@ -9501,6 +9951,10 @@
         <v>2.0879500000000002</v>
       </c>
       <c r="H69"/>
+      <c r="M69">
+        <f>LOG10(3.994328693)</f>
+        <v>0.60144380006461717</v>
+      </c>
       <c r="O69" s="10"/>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
@@ -9537,6 +9991,10 @@
         <v>2.2751999999999999</v>
       </c>
       <c r="H71"/>
+      <c r="M71">
+        <f>LOG10(3.993186401)</f>
+        <v>0.60131958343156777</v>
+      </c>
       <c r="O71" s="10"/>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
@@ -9583,6 +10041,10 @@
         <f>LOG10(232.642858)</f>
         <v>2.3666897244867378</v>
       </c>
+      <c r="M73">
+        <f>LOG10(8.444519779)</f>
+        <v>0.92657495725097339</v>
+      </c>
       <c r="O73" s="10"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
@@ -9613,6 +10075,10 @@
         <v>2.2058800000000001</v>
       </c>
       <c r="H75"/>
+      <c r="M75">
+        <f>LOG10(4.808374287)</f>
+        <v>0.68199826607705716</v>
+      </c>
       <c r="O75" s="10"/>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
@@ -9649,6 +10115,10 @@
         <v>2.84788</v>
       </c>
       <c r="H77"/>
+      <c r="M77">
+        <f>LOG10(9.736055533)</f>
+        <v>0.98838304237963814</v>
+      </c>
       <c r="O77" s="10"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
@@ -9701,6 +10171,10 @@
         <v>2.5167199999999998</v>
       </c>
       <c r="H80"/>
+      <c r="M80">
+        <f>LOG10(6.170551584)</f>
+        <v>0.79032398723916319</v>
+      </c>
       <c r="O80" s="10"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
@@ -9932,6 +10406,10 @@
         <v>3.0066999999999999</v>
       </c>
       <c r="H94"/>
+      <c r="M94">
+        <f>LOG10(9.123023933)</f>
+        <v>0.96013881417720048</v>
+      </c>
       <c r="O94" s="10"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
@@ -10184,6 +10662,10 @@
         <v>3.5022199999999999</v>
       </c>
       <c r="H111"/>
+      <c r="M111">
+        <f>LOG10(14.501266966)</f>
+        <v>1.1614059479111796</v>
+      </c>
       <c r="O111" s="10"/>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.25">
@@ -10236,6 +10718,10 @@
         <v>3.9498099999999998</v>
       </c>
       <c r="H114"/>
+      <c r="M114">
+        <f>LOG10(24.59653992)</f>
+        <v>1.3908740176992924</v>
+      </c>
       <c r="O114" s="10"/>
     </row>
     <row r="115" spans="2:15" x14ac:dyDescent="0.25">
@@ -10276,29 +10762,23 @@
     </row>
     <row r="117" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B117">
-        <v>50653</v>
+        <v>45369</v>
       </c>
       <c r="C117"/>
       <c r="D117"/>
       <c r="E117"/>
       <c r="F117"/>
       <c r="G117"/>
-      <c r="H117">
-        <v>3.97126</v>
-      </c>
-      <c r="L117">
-        <f>LOG10(19.431127)</f>
-        <v>1.2884979902903051</v>
-      </c>
-      <c r="N117">
-        <f>LOG10(21.867876)</f>
-        <v>1.3398066025952082</v>
+      <c r="H117"/>
+      <c r="M117">
+        <f>LOG10(35.086501703)</f>
+        <v>1.5451400690754507</v>
       </c>
       <c r="O117" s="10"/>
     </row>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B118">
-        <v>64000</v>
+        <v>50653</v>
       </c>
       <c r="C118"/>
       <c r="D118"/>
@@ -10306,43 +10786,37 @@
       <c r="F118"/>
       <c r="G118"/>
       <c r="H118">
-        <v>4.2911099999999998</v>
+        <v>3.97126</v>
       </c>
       <c r="L118">
-        <f>LOG10(26.628915)</f>
-        <v>1.4253534713915326</v>
+        <f>LOG10(19.431127)</f>
+        <v>1.2884979902903051</v>
       </c>
       <c r="N118">
-        <f>LOG10(29.583712)</f>
-        <v>1.4710526659412606</v>
+        <f>LOG10(21.867876)</f>
+        <v>1.3398066025952082</v>
       </c>
       <c r="O118" s="10"/>
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B119">
-        <v>74088</v>
+        <v>55225</v>
       </c>
       <c r="C119"/>
       <c r="D119"/>
       <c r="E119"/>
       <c r="F119"/>
       <c r="G119"/>
-      <c r="H119">
-        <v>4.4571699999999996</v>
-      </c>
-      <c r="L119">
-        <f>LOG10(32.613322)</f>
-        <v>1.5133950383885446</v>
-      </c>
-      <c r="N119">
-        <f>LOG10(35.725403)</f>
-        <v>1.5529771365445766</v>
+      <c r="H119"/>
+      <c r="M119">
+        <f>LOG10(47.203422647)</f>
+        <v>1.6739734897954159</v>
       </c>
       <c r="O119" s="10"/>
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B120">
-        <v>85184</v>
+        <v>64000</v>
       </c>
       <c r="C120"/>
       <c r="D120"/>
@@ -10350,43 +10824,37 @@
       <c r="F120"/>
       <c r="G120"/>
       <c r="H120">
-        <v>4.5895700000000001</v>
+        <v>4.2911099999999998</v>
       </c>
       <c r="L120">
-        <f>LOG10(34.527966)</f>
-        <v>1.5381709953493281</v>
+        <f>LOG10(26.628915)</f>
+        <v>1.4253534713915326</v>
       </c>
       <c r="N120">
-        <f>LOG10(91.245534)</f>
-        <v>1.960211617165541</v>
+        <f>LOG10(29.583712)</f>
+        <v>1.4710526659412606</v>
       </c>
       <c r="O120" s="10"/>
     </row>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B121">
-        <v>91125</v>
+        <v>65025</v>
       </c>
       <c r="C121"/>
       <c r="D121"/>
       <c r="E121"/>
       <c r="F121"/>
       <c r="G121"/>
-      <c r="H121">
-        <v>4.6817700000000002</v>
-      </c>
-      <c r="L121">
-        <f>LOG10(34.134635)</f>
-        <v>1.5331952633226487</v>
-      </c>
-      <c r="N121">
-        <f>LOG10(146.876535)</f>
-        <v>2.1669524184314453</v>
+      <c r="H121"/>
+      <c r="M121">
+        <f>LOG10(49.623899971)</f>
+        <v>1.6956908927319843</v>
       </c>
       <c r="O121" s="10"/>
     </row>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B122">
-        <v>103823</v>
+        <v>74088</v>
       </c>
       <c r="C122"/>
       <c r="D122"/>
@@ -10394,19 +10862,21 @@
       <c r="F122"/>
       <c r="G122"/>
       <c r="H122">
-        <v>4.7963300000000002</v>
-      </c>
-      <c r="L122" s="8">
-        <v>2.1273930000000001</v>
-      </c>
-      <c r="N122" s="8">
-        <v>2.499571</v>
+        <v>4.4571699999999996</v>
+      </c>
+      <c r="L122">
+        <f>LOG10(32.613322)</f>
+        <v>1.5133950383885446</v>
+      </c>
+      <c r="N122">
+        <f>LOG10(35.725403)</f>
+        <v>1.5529771365445766</v>
       </c>
       <c r="O122" s="10"/>
     </row>
     <row r="123" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B123">
-        <v>100489</v>
+        <v>75076</v>
       </c>
       <c r="C123"/>
       <c r="D123"/>
@@ -10414,17 +10884,15 @@
       <c r="F123"/>
       <c r="G123"/>
       <c r="H123"/>
-      <c r="K123" s="8">
-        <v>1.7864169999999999</v>
-      </c>
-      <c r="M123" s="8">
-        <v>1.875286</v>
+      <c r="M123">
+        <f>LOG10(50.352247452)</f>
+        <v>1.7020188598790844</v>
       </c>
       <c r="O123" s="10"/>
     </row>
     <row r="124" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B124">
-        <v>205379</v>
+        <v>85184</v>
       </c>
       <c r="C124"/>
       <c r="D124"/>
@@ -10432,68 +10900,220 @@
       <c r="F124"/>
       <c r="G124"/>
       <c r="H124">
-        <v>5.67401</v>
+        <v>4.5895700000000001</v>
+      </c>
+      <c r="L124">
+        <f>LOG10(34.527966)</f>
+        <v>1.5381709953493281</v>
+      </c>
+      <c r="N124">
+        <f>LOG10(91.245534)</f>
+        <v>1.960211617165541</v>
       </c>
       <c r="O124" s="10"/>
     </row>
     <row r="125" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B125">
-        <v>300763</v>
+        <v>85264</v>
       </c>
       <c r="C125"/>
       <c r="D125"/>
       <c r="E125"/>
       <c r="F125"/>
       <c r="G125"/>
-      <c r="H125">
+      <c r="H125"/>
+      <c r="M125">
+        <f>LOG10(55.180770926)</f>
+        <v>1.7417877636779429</v>
+      </c>
+      <c r="O125" s="10"/>
+    </row>
+    <row r="126" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>91125</v>
+      </c>
+      <c r="C126"/>
+      <c r="D126"/>
+      <c r="E126"/>
+      <c r="F126"/>
+      <c r="G126"/>
+      <c r="H126">
+        <v>4.6817700000000002</v>
+      </c>
+      <c r="L126">
+        <f>LOG10(34.134635)</f>
+        <v>1.5331952633226487</v>
+      </c>
+      <c r="N126">
+        <f>LOG10(146.876535)</f>
+        <v>2.1669524184314453</v>
+      </c>
+      <c r="O126" s="10"/>
+    </row>
+    <row r="127" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>95481</v>
+      </c>
+      <c r="C127"/>
+      <c r="D127"/>
+      <c r="E127"/>
+      <c r="F127"/>
+      <c r="G127"/>
+      <c r="H127"/>
+      <c r="M127">
+        <f>LOG10(77.473349353)</f>
+        <v>1.8891523319326773</v>
+      </c>
+      <c r="O127" s="10"/>
+    </row>
+    <row r="128" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>100489</v>
+      </c>
+      <c r="C128"/>
+      <c r="D128"/>
+      <c r="E128"/>
+      <c r="F128"/>
+      <c r="G128"/>
+      <c r="H128"/>
+      <c r="K128" s="8">
+        <v>1.7864169999999999</v>
+      </c>
+      <c r="M128" s="8">
+        <v>1.875286</v>
+      </c>
+      <c r="O128" s="10"/>
+    </row>
+    <row r="129" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>103823</v>
+      </c>
+      <c r="C129"/>
+      <c r="D129"/>
+      <c r="E129"/>
+      <c r="F129"/>
+      <c r="G129"/>
+      <c r="H129">
+        <v>4.7963300000000002</v>
+      </c>
+      <c r="L129" s="8">
+        <v>2.1273930000000001</v>
+      </c>
+      <c r="N129" s="8">
+        <v>2.499571</v>
+      </c>
+      <c r="O129" s="10"/>
+    </row>
+    <row r="130" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>105625</v>
+      </c>
+      <c r="C130"/>
+      <c r="D130"/>
+      <c r="E130"/>
+      <c r="F130"/>
+      <c r="G130"/>
+      <c r="H130"/>
+      <c r="L130" s="8"/>
+      <c r="M130">
+        <f>LOG10(79.383290971)</f>
+        <v>1.8997290993698215</v>
+      </c>
+      <c r="N130" s="8"/>
+      <c r="O130" s="10"/>
+    </row>
+    <row r="131" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>205209</v>
+      </c>
+      <c r="C131"/>
+      <c r="D131"/>
+      <c r="E131"/>
+      <c r="F131"/>
+      <c r="G131"/>
+      <c r="H131"/>
+      <c r="L131" s="8"/>
+      <c r="M131">
+        <f>LOG10(149.866024681)</f>
+        <v>2.1757031874447921</v>
+      </c>
+      <c r="N131" s="8"/>
+      <c r="O131" s="10"/>
+    </row>
+    <row r="132" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>205379</v>
+      </c>
+      <c r="C132"/>
+      <c r="D132"/>
+      <c r="E132"/>
+      <c r="F132"/>
+      <c r="G132"/>
+      <c r="H132">
+        <v>5.67401</v>
+      </c>
+      <c r="M132" s="10"/>
+      <c r="O132" s="10"/>
+    </row>
+    <row r="133" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>300763</v>
+      </c>
+      <c r="C133"/>
+      <c r="D133"/>
+      <c r="E133"/>
+      <c r="F133"/>
+      <c r="G133"/>
+      <c r="H133">
         <v>6.59</v>
       </c>
-      <c r="O125" s="10"/>
-    </row>
-    <row r="126" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D126"/>
-    </row>
-    <row r="127" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D127"/>
-    </row>
-    <row r="128" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D128"/>
-    </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D129"/>
-    </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D130"/>
-    </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D131"/>
-    </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D132"/>
-    </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D133"/>
-    </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="M133" s="10"/>
+      <c r="O133" s="10"/>
+    </row>
+    <row r="134" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D134"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D135"/>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D136"/>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D137"/>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D138"/>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D139"/>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D140"/>
+    </row>
+    <row r="141" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D141"/>
+    </row>
+    <row r="142" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D142"/>
+    </row>
+    <row r="143" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D143"/>
+    </row>
+    <row r="144" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D144"/>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D145"/>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D146"/>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D147"/>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D148"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
transferred report to docx file
</commit_message>
<xml_diff>
--- a/Project2/report.xlsx
+++ b/Project2/report.xlsx
@@ -3444,11 +3444,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="355682448"/>
-        <c:axId val="355684016"/>
+        <c:axId val="354432872"/>
+        <c:axId val="354433656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="355682448"/>
+        <c:axId val="354432872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3547,7 +3547,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="355684016"/>
+        <c:crossAx val="354433656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3555,7 +3555,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="355684016"/>
+        <c:axId val="354433656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3662,7 +3662,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="355682448"/>
+        <c:crossAx val="354432872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6905,12 +6905,12 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="355683232"/>
-        <c:axId val="357348168"/>
+        <c:axId val="354434048"/>
+        <c:axId val="354434440"/>
         <c:extLst/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="355683232"/>
+        <c:axId val="354434048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7009,7 +7009,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="357348168"/>
+        <c:crossAx val="354434440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7017,7 +7017,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="357348168"/>
+        <c:axId val="354434440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7124,7 +7124,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="355683232"/>
+        <c:crossAx val="354434048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8295,16 +8295,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>171449</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8325,16 +8325,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>314324</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>161923</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8621,9 +8621,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L129" sqref="L129"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>